<commit_message>
Fix typo in ProtectedArea and TopographicalElement
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules_v1.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6BBC61-2173-4622-A9E8-5C320224CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA51C45-A0CE-48B1-AE15-F9E3177AD2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="16" activeTab="25" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="16" activeTab="23" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL3 Extra Rules" sheetId="1" r:id="rId1"/>
@@ -5759,8 +5759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2764A8-90B0-4CAB-A949-0A9B643E9D1B}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7326,7 +7326,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8604,7 +8604,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9262,7 +9262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F037272-C335-49D9-940E-9503A9473373}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -9736,7 +9736,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10395,7 +10395,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10710,7 +10710,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11195,7 +11195,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11459,8 +11459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2626C4B8-913D-4090-B23B-9F41B06EEF20}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11768,7 +11768,7 @@
         <v>103</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>59</v>
@@ -11833,7 +11833,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12121,7 +12121,7 @@
         <v>103</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>59</v>
@@ -12165,8 +12165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B0875E-4BBC-4337-B179-D80DFA58D9BF}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12499,7 +12499,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13051,8 +13051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D942B28-BE2C-4879-B771-95BEB360A522}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13824,7 +13824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEEBB16-5094-4A68-A615-43B0896E521F}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
@@ -14777,8 +14777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B140CE-B260-4273-B7CB-D8C81EBB6EBD}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15550,8 +15550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10101923-3348-4496-9274-4B73928D2D00}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16343,8 +16343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0213BD-F2E7-42B7-80C7-ACC383C2E599}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17946,15 +17946,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -18214,15 +18205,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDFEA48-FAC4-456B-938A-80A9A9627A87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18240,4 +18232,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix typo in rules for TopographicalElement
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules_v1.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA51C45-A0CE-48B1-AE15-F9E3177AD2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7547C9-130F-4B6A-B63E-4A45E63DB562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="16" activeTab="23" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="15" activeTab="24" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL3 Extra Rules" sheetId="1" r:id="rId1"/>
@@ -11459,8 +11459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2626C4B8-913D-4090-B23B-9F41B06EEF20}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11832,8 +11832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52607BE3-DC00-46A5-B151-3ABD17EEE6D5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12021,7 +12021,7 @@
         <v>101</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>59</v>
@@ -12041,7 +12041,7 @@
         <v>102</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>59</v>
@@ -12121,7 +12121,7 @@
         <v>103</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>59</v>
@@ -12141,7 +12141,7 @@
         <v>104</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>59</v>

</xml_diff>